<commit_message>
Remove some out-of-date junk, and update todo list.
</commit_message>
<xml_diff>
--- a/LoftyCAD TODO list.xlsx
+++ b/LoftyCAD TODO list.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Giles\LoftyCAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\LoftyCAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,86 +24,17 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>LoftyCAD Order of March</t>
   </si>
   <si>
-    <t>Rect faces, volumes</t>
-  </si>
-  <si>
-    <t>Polygon faces, volumes</t>
-  </si>
-  <si>
-    <t>2a</t>
-  </si>
-  <si>
-    <t>circles, arcs and beziers are special cases of polygon edges</t>
-  </si>
-  <si>
-    <t>2b</t>
-  </si>
-  <si>
-    <t>Joining edges to other edges, and closing to make a face</t>
-  </si>
-  <si>
-    <t>Decisions about shading/highlight/select coloring</t>
-  </si>
-  <si>
-    <t>3a</t>
-  </si>
-  <si>
-    <t>lighting option for rendering</t>
-  </si>
-  <si>
-    <t>Writing out and reading back</t>
-  </si>
-  <si>
-    <t>4a</t>
-  </si>
-  <si>
-    <t>the Undo stack (serialise for every change)</t>
-  </si>
-  <si>
     <t>Picking (type priority overrides frontmost)</t>
   </si>
   <si>
-    <t>5a</t>
-  </si>
-  <si>
-    <t>line-line nearest intersection</t>
-  </si>
-  <si>
     <t>Selection</t>
   </si>
   <si>
-    <t>6a</t>
-  </si>
-  <si>
-    <t>moving a selection</t>
-  </si>
-  <si>
-    <t>6b</t>
-  </si>
-  <si>
-    <t>6c</t>
-  </si>
-  <si>
-    <t>scaling/rotation of a selection</t>
-  </si>
-  <si>
-    <t>measures and construction edges</t>
-  </si>
-  <si>
-    <t>Extruding</t>
-  </si>
-  <si>
-    <t>copy/paste/delete a selection - deep-copy</t>
-  </si>
-  <si>
-    <t>Triangulation and export of STL</t>
-  </si>
-  <si>
     <t>Job</t>
   </si>
   <si>
@@ -113,31 +44,46 @@
     <t>Sub-goals</t>
   </si>
   <si>
-    <t>Buttons</t>
-  </si>
-  <si>
-    <t>Buttons and help text</t>
-  </si>
-  <si>
-    <t>Menu items</t>
-  </si>
-  <si>
-    <t>How to do random reading in undo file</t>
-  </si>
-  <si>
-    <t>deep-copy an edge, face or volume</t>
-  </si>
-  <si>
     <t>TODO lists</t>
   </si>
   <si>
-    <t>facing planes, interface niggles</t>
-  </si>
-  <si>
-    <t>Thick lines, dotted lines</t>
-  </si>
-  <si>
-    <t>Button/icons, dotted lines, 2D arrows</t>
+    <t>* rework picking so small object sitting in large one gets priority</t>
+  </si>
+  <si>
+    <t>dotted lines, 2D arrows</t>
+  </si>
+  <si>
+    <t>* scaling/rotation of a selection</t>
+  </si>
+  <si>
+    <t>Lofting, and other ways of specifying things</t>
+  </si>
+  <si>
+    <t>* sticky rulers, standoff measurements</t>
+  </si>
+  <si>
+    <t>* picking edges on faces not reliable</t>
+  </si>
+  <si>
+    <t>Measures and construction edges</t>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>* fix bugs in grouping when unlocked at various levels - only parents get grouped</t>
+  </si>
+  <si>
+    <t>Object tree view</t>
+  </si>
+  <si>
+    <t>* fix bug where wrong object gets highlighted when in group</t>
+  </si>
+  <si>
+    <t>* be able to do right-click things on the object view</t>
+  </si>
+  <si>
+    <t>Wait-cursor and/or progress bar when building mesh</t>
   </si>
 </sst>
 </file>
@@ -465,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,186 +430,116 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>4</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
+      <c r="A3" s="2">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>19</v>
+      </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="B5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>30</v>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B8" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
       <c r="B10" t="s">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
       <c r="B12" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" t="s">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
+      <c r="B15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16" t="s">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>19</v>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
-      </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>7</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>8</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <v>9</v>
-      </c>
-      <c r="B21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22">
         <v>10</v>
-      </c>
-      <c r="B22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Put temp files in the temp directory, and use module filename to find the html directory. This keeps writes out of the program files directory when the installer is used.
</commit_message>
<xml_diff>
--- a/LoftyCAD TODO list.xlsx
+++ b/LoftyCAD TODO list.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>LoftyCAD Order of March</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>Wait-cursor and/or progress bar when building mesh</t>
+  </si>
+  <si>
+    <t>Constraints (point-edge, face-face, perp, parallel, etc)</t>
   </si>
 </sst>
 </file>
@@ -411,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -542,6 +545,14 @@
         <v>10</v>
       </c>
     </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>21</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>